<commit_message>
Update data files and add new project files
</commit_message>
<xml_diff>
--- a/data/пример ответов.xlsx
+++ b/data/пример ответов.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDSko\Desktop\DevAI\HayAutoGrade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC2DCE-25F1-4343-BE41-1A5807EC015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A701749-D4E3-46F1-8DE9-EFAC68FBCB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{820F74FF-0D2A-4AEA-99FE-F9819A7973DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{820F74FF-0D2A-4AEA-99FE-F9819A7973DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>9. Какой уровень планирования и организации соответствует вашей роли?</t>
   </si>
   <si>
-    <t>Стратегическое планирование развития направления AI на квартал и год. Организация спринтов (2 недели), распределение задач между разработчиками. Контроль разработки AI-агентов от идеи до продакшена — архитектура, качество кода, тестирование, деплой.</t>
-  </si>
-  <si>
     <t>10. Какой уровень экспертизы и глубины знаний требуется для этой должности?</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Высокая степень самостоятельности: принятие решений по архитектуре решений, выбору технологий и формированию команды.</t>
+  </si>
+  <si>
+    <t>Организация спринтов (2 недели), распределение задач между разработчиками. Контроль разработки AI-агентов от идеи до продакшена — архитектура, качество кода, тестирование, деплой.</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFAC17E-4BBE-48F2-8FB3-0F11BAA5C23A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,7 +696,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="87" x14ac:dyDescent="0.35">
@@ -707,60 +707,60 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>